<commit_message>
modified the previous errors and should be good
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Batch19TestData1.xlsx
+++ b/src/test/resources/testData/Batch19TestData1.xlsx
@@ -63,7 +63,7 @@
     <t>/Users/shpendpllana/Desktop/NYC.jpg</t>
   </si>
   <si>
-    <t>ane98</t>
+    <t>ane981</t>
   </si>
   <si>
     <t>Hum@nhrm123</t>
@@ -78,7 +78,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>johnTheJOe12</t>
+    <t>johnTheJOe121</t>
   </si>
   <si>
     <t>Laura</t>
@@ -90,7 +90,7 @@
     <t>Ricarso</t>
   </si>
   <si>
-    <t>auraLAura90</t>
+    <t>auraLAura901</t>
   </si>
   <si>
     <t>Sarah</t>
@@ -102,7 +102,7 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>saratheS1</t>
+    <t>saratheS11</t>
   </si>
   <si>
     <t>Linda</t>
@@ -114,7 +114,7 @@
     <t>Christos</t>
   </si>
   <si>
-    <t>lindaBone123</t>
+    <t>lindaBone1231</t>
   </si>
   <si>
     <t>Joe</t>
@@ -126,7 +126,7 @@
     <t>Partiz</t>
   </si>
   <si>
-    <t>johnTrucker73</t>
+    <t>johnTrucker731</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
worked around all test cases and fixed the scrip
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Batch19TestData1.xlsx
+++ b/src/test/resources/testData/Batch19TestData1.xlsx
@@ -63,7 +63,7 @@
     <t>/Users/shpendpllana/Desktop/NYC.jpg</t>
   </si>
   <si>
-    <t>JJANE</t>
+    <t>janeTheGem</t>
   </si>
   <si>
     <t>Hum@nhrm123</t>
@@ -78,7 +78,7 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>john09</t>
+    <t>johntheGoat</t>
   </si>
   <si>
     <t>Laura</t>
@@ -90,7 +90,7 @@
     <t>Ricarso</t>
   </si>
   <si>
-    <t>adENA</t>
+    <t>lauraTheRainbow</t>
   </si>
   <si>
     <t>Sarah</t>
@@ -102,7 +102,7 @@
     <t>Brown</t>
   </si>
   <si>
-    <t>sarat3ITA</t>
+    <t>saraThegold</t>
   </si>
   <si>
     <t>Linda</t>
@@ -114,7 +114,7 @@
     <t>Christos</t>
   </si>
   <si>
-    <t>linda11EAD1</t>
+    <t>lindaArrio</t>
   </si>
   <si>
     <t>Joe</t>
@@ -126,7 +126,7 @@
     <t>Partiz</t>
   </si>
   <si>
-    <t>johnggDDS</t>
+    <t>joeBear</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
pushing the changes I have made locally and waiting to jenkins reports
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Batch19TestData1.xlsx
+++ b/src/test/resources/testData/Batch19TestData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28160" windowHeight="14420"/>
+    <workbookView windowWidth="32000" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>firstName</t>
   </si>
@@ -51,19 +51,19 @@
     <t>confirmPassword</t>
   </si>
   <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>XHIXHI</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
-    <t>/Users/shpendpllana/Desktop/NYC.jpg</t>
-  </si>
-  <si>
-    <t>janeTheGem</t>
+    <t>Lil</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Rapper</t>
+  </si>
+  <si>
+    <t>/Users/shpendpllana/Desktop/PANDA.jpeg</t>
+  </si>
+  <si>
+    <t>lilTheBest</t>
   </si>
   <si>
     <t>Hum@nhrm123</t>
@@ -72,61 +72,70 @@
     <t>John</t>
   </si>
   <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>johntheGoat</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>LR</t>
-  </si>
-  <si>
-    <t>Ricarso</t>
-  </si>
-  <si>
-    <t>lauraTheRainbow</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>SRB</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>saraThegold</t>
-  </si>
-  <si>
-    <t>Linda</t>
-  </si>
-  <si>
-    <t>LCH</t>
-  </si>
-  <si>
-    <t>Christos</t>
-  </si>
-  <si>
-    <t>lindaArrio</t>
-  </si>
-  <si>
-    <t>Joe</t>
-  </si>
-  <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>Partiz</t>
-  </si>
-  <si>
-    <t>joeBear</t>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Goat</t>
+  </si>
+  <si>
+    <t>bones123</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>lyricalist</t>
+  </si>
+  <si>
+    <t>emcylopedi</t>
+  </si>
+  <si>
+    <t>m&amp;m</t>
+  </si>
+  <si>
+    <t>50cent</t>
+  </si>
+  <si>
+    <t>gangsta</t>
+  </si>
+  <si>
+    <t>realG</t>
+  </si>
+  <si>
+    <t>50gold</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
+    <t>debugger95</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>thebestCareer</t>
+  </si>
+  <si>
+    <t>NQ</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>TRADE</t>
+  </si>
+  <si>
+    <t>lifeChanger</t>
   </si>
 </sst>
 </file>
@@ -1106,13 +1115,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="17.703125" customWidth="1"/>
     <col min="2" max="2" width="14.84375" customWidth="1"/>
@@ -1269,18 +1278,41 @@
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1298,6 +1330,8 @@
     <hyperlink ref="G6" r:id="rId1" display="Hum@nhrm123"/>
     <hyperlink ref="F7" r:id="rId1" display="Hum@nhrm123"/>
     <hyperlink ref="G7" r:id="rId1" display="Hum@nhrm123"/>
+    <hyperlink ref="F8" r:id="rId1" display="Hum@nhrm123"/>
+    <hyperlink ref="G8" r:id="rId1" display="Hum@nhrm123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>